<commit_message>
Update mapping of environmental flows
</commit_message>
<xml_diff>
--- a/dev/material_flows_ecoinvent.xlsx
+++ b/dev/material_flows_ecoinvent.xlsx
@@ -2151,7 +2151,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:I247" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:I247" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:I247"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Activity"/>
@@ -2181,7 +2181,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H235" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H235" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:H235"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Activity"/>
@@ -2463,7 +2463,7 @@
   <dimension ref="A1:W247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H221" sqref="H221"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>